<commit_message>
Changed my fetching code
Changed the code to fetch blocks and entities, perfected code to fetch data for player
Also fixed some issues where it wouldn't fetch the sprite for the GameScene
</commit_message>
<xml_diff>
--- a/Game_Engine/Shared/Resources/tables/Sprites.xlsx
+++ b/Game_Engine/Shared/Resources/tables/Sprites.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphaelgournay/Documents/GitHub/Physics-Engine/Physics_Engine/Shared/Resources/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphaelgournay/Documents/GitHub/Physics-Engine/Game_Engine/Shared/Resources/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>block</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>sprites/player/p1</t>
+  </si>
+  <si>
+    <t>sprites/enemy/e1</t>
+  </si>
+  <si>
+    <t>sprites/enemy/e2</t>
+  </si>
+  <si>
+    <t>blocks/b1</t>
+  </si>
+  <si>
+    <t>blocks/b2</t>
+  </si>
+  <si>
+    <t>blocks/s1</t>
+  </si>
+  <si>
+    <t>blocks/s2</t>
+  </si>
+  <si>
+    <t>blocks/r1</t>
   </si>
 </sst>
 </file>
@@ -410,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,6 +590,35 @@
         <v>2</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor fixes and Added collision detection
Made some fixes that allowed me to fetch the height of the sprites from the table ( it didn't work before) And added some basic collision detection whilst moving
</commit_message>
<xml_diff>
--- a/Game_Engine/Shared/Resources/tables/Sprites.xlsx
+++ b/Game_Engine/Shared/Resources/tables/Sprites.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>blocks/r1</t>
+  </si>
+  <si>
+    <t>yShift</t>
+  </si>
+  <si>
+    <t>sprite height</t>
   </si>
 </sst>
 </file>
@@ -437,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -464,8 +470,14 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -484,8 +496,15 @@
       <c r="F2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -504,8 +523,14 @@
       <c r="F3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -524,8 +549,14 @@
       <c r="F4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -544,8 +575,14 @@
       <c r="F5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -564,8 +601,14 @@
       <c r="F6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -584,8 +627,14 @@
       <c r="F7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -604,8 +653,14 @@
       <c r="F8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -623,6 +678,12 @@
       </c>
       <c r="F9" t="s">
         <v>31</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made upgrades to the detection of objects
The system is now able to make the character fall to the bottom when not on a platform, and Change its zPosition so that it appears to be behind objects when on differenct floors to them when necessary
</commit_message>
<xml_diff>
--- a/Game_Engine/Shared/Resources/tables/Sprites.xlsx
+++ b/Game_Engine/Shared/Resources/tables/Sprites.xlsx
@@ -446,7 +446,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,7 +596,7 @@
         <v>22</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
@@ -648,7 +648,7 @@
         <v>22</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>

</xml_diff>